<commit_message>
Metricas Vector actualizacion lineas atributos, constructores. metricas sel  actualizacion lineas atributos, constructores - ademas agregado dos metodos al final.
</commit_message>
<xml_diff>
--- a/Preparacion De La Prueba/Lote De Prueba/Documentacion/Sel/Sel - Planilla de Métricas V2.1.xlsx
+++ b/Preparacion De La Prueba/Lote De Prueba/Documentacion/Sel/Sel - Planilla de Métricas V2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgIII\BranchGus\Documentacion\Sel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgIII\Reentrega\Preparacion De La Prueba\Lote De Prueba\Documentacion\Sel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -140,6 +140,12 @@
   <si>
     <t>calcularError()</t>
   </si>
+  <si>
+    <t>tieneAtributosIncompletos()</t>
+  </si>
+  <si>
+    <t>escribirArchivoSalida()</t>
+  </si>
 </sst>
 </file>
 
@@ -258,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -762,11 +768,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -981,9 +1000,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1018,29 +1034,51 @@
     <xf numFmtId="20" fontId="7" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1062,41 +1100,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,7 +1303,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$36:$B$41</c:f>
+              <c:f>Métricas!$B$39:$B$44</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1290,27 +1329,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$F$36:$F$41</c:f>
+              <c:f>Métricas!$F$39:$F$44</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.096385542168679E-2</c:v>
+                  <c:v>3.8288288288288341E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48192771084337327</c:v>
+                  <c:v>0.45045045045045046</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.096385542168679E-2</c:v>
+                  <c:v>3.8288288288288341E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10120481927710845</c:v>
+                  <c:v>9.4594594594594641E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8192771084337345E-2</c:v>
+                  <c:v>6.9819819819819842E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.28674698795180731</c:v>
+                  <c:v>0.30855855855855829</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1361,13 +1400,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1433,7 +1472,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1468,7 +1507,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1653,10 +1692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1675,23 +1714,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="111"/>
-      <c r="D1" s="118" t="s">
+      <c r="C1" s="86"/>
+      <c r="D1" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1735,12 +1774,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="89"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -1866,12 +1905,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1908,15 +1947,15 @@
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="110"/>
-      <c r="G8" s="111"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="111"/>
-      <c r="L8" s="111"/>
-      <c r="M8" s="111"/>
-      <c r="N8" s="111"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -1941,19 +1980,19 @@
       <c r="D9" s="25">
         <v>0.48472222222222222</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="84">
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>0.13888888888888884</v>
       </c>
-      <c r="F9" s="112"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="111"/>
-      <c r="M9" s="111"/>
-      <c r="N9" s="111"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -1997,12 +2036,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="87"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2039,15 +2078,15 @@
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="110"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
-      <c r="L12" s="111"/>
-      <c r="M12" s="111"/>
-      <c r="N12" s="111"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2076,15 +2115,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>1.1805555555555569E-2</v>
       </c>
-      <c r="F13" s="112"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2128,21 +2167,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="86"/>
-      <c r="N15" s="87"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="89"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2158,31 +2197,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="C16" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="103" t="s">
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="104"/>
-      <c r="H16" s="102" t="s">
+      <c r="G16" s="109"/>
+      <c r="H16" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="103" t="s">
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="L16" s="104"/>
-      <c r="M16" s="105" t="s">
+      <c r="L16" s="109"/>
+      <c r="M16" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="N16" s="98" t="s">
+      <c r="N16" s="103" t="s">
         <v>5</v>
       </c>
       <c r="O16" s="7"/>
@@ -2200,10 +2239,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="97"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
       <c r="F17" s="26" t="s">
         <v>15</v>
       </c>
@@ -2225,8 +2264,8 @@
       <c r="L17" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M17" s="106"/>
-      <c r="N17" s="99"/>
+      <c r="M17" s="111"/>
+      <c r="N17" s="104"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2243,14 +2282,13 @@
     <row r="18" spans="1:26">
       <c r="A18" s="15"/>
       <c r="B18" s="30">
-        <f t="shared" ref="B18:B24" si="0">ROW($B18)-16</f>
-        <v>2</v>
+        <v>1</v>
       </c>
-      <c r="C18" s="90" t="s">
+      <c r="C18" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2264,7 +2302,7 @@
         <v>0.54513888888888895</v>
       </c>
       <c r="J18" s="35">
-        <f t="shared" ref="J18:J22" si="1">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
+        <f t="shared" ref="J18:J24" si="0">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
         <v>2.7777777777777901E-2</v>
       </c>
       <c r="K18" s="36">
@@ -2274,10 +2312,10 @@
         <v>0</v>
       </c>
       <c r="M18" s="38">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="N18" s="39">
-        <f t="shared" ref="N18:N24" si="2">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
+        <f t="shared" ref="N18:N27" si="1">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
         <v>2.7777777777777901E-2</v>
       </c>
       <c r="O18" s="15"/>
@@ -2296,14 +2334,13 @@
     <row r="19" spans="1:26">
       <c r="A19" s="15"/>
       <c r="B19" s="30">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="C19" s="100" t="s">
+      <c r="C19" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
       <c r="F19" s="31">
         <v>10</v>
       </c>
@@ -2317,7 +2354,7 @@
         <v>0.6069444444444444</v>
       </c>
       <c r="J19" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="K19" s="36">
@@ -2330,7 +2367,7 @@
         <v>8</v>
       </c>
       <c r="N19" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="O19" s="15"/>
@@ -2349,14 +2386,13 @@
     <row r="20" spans="1:26">
       <c r="A20" s="15"/>
       <c r="B20" s="30">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
       <c r="F20" s="31">
         <v>10</v>
       </c>
@@ -2370,7 +2406,7 @@
         <v>0.60972222222222217</v>
       </c>
       <c r="J20" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.0833333333332149E-3</v>
       </c>
       <c r="K20" s="36">
@@ -2383,7 +2419,7 @@
         <v>7</v>
       </c>
       <c r="N20" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.0833333333332149E-3</v>
       </c>
       <c r="O20" s="15"/>
@@ -2402,14 +2438,13 @@
     <row r="21" spans="1:26">
       <c r="A21" s="15"/>
       <c r="B21" s="30">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
       <c r="F21" s="31">
         <v>60</v>
       </c>
@@ -2423,20 +2458,20 @@
         <v>0.62986111111111109</v>
       </c>
       <c r="J21" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5972222222222276E-2</v>
       </c>
       <c r="K21" s="36">
         <v>1</v>
       </c>
-      <c r="L21" s="81">
+      <c r="L21" s="80">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="M21" s="38">
         <v>16</v>
       </c>
       <c r="N21" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.94444444444445E-2</v>
       </c>
       <c r="O21" s="15"/>
@@ -2452,451 +2487,492 @@
       <c r="Y21" s="22"/>
       <c r="Z21" s="22"/>
     </row>
-    <row r="22" spans="1:26" s="80" customFormat="1" ht="15" customHeight="1">
+    <row r="22" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="71"/>
-      <c r="B22" s="72">
-        <f t="shared" si="0"/>
-        <v>6</v>
+      <c r="B22" s="30">
+        <v>5</v>
       </c>
-      <c r="C22" s="101" t="s">
+      <c r="C22" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="82">
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="81">
         <v>15</v>
       </c>
-      <c r="G22" s="83">
+      <c r="G22" s="82">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H22" s="84">
+      <c r="H22" s="83">
         <v>6.5972222222222224E-2</v>
       </c>
-      <c r="I22" s="73">
+      <c r="I22" s="72">
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="J22" s="74">
-        <f t="shared" si="1"/>
+      <c r="J22" s="73">
+        <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="K22" s="75">
+      <c r="K22" s="74">
         <v>1</v>
       </c>
-      <c r="L22" s="76">
+      <c r="L22" s="75">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="M22" s="77">
+      <c r="M22" s="76">
         <v>11</v>
       </c>
       <c r="N22" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O22" s="71"/>
-      <c r="P22" s="78"/>
-      <c r="Q22" s="79"/>
-      <c r="R22" s="79"/>
-      <c r="S22" s="79"/>
-      <c r="T22" s="79"/>
-      <c r="U22" s="79"/>
-      <c r="V22" s="79"/>
-      <c r="W22" s="79"/>
-      <c r="X22" s="79"/>
-      <c r="Y22" s="79"/>
-      <c r="Z22" s="79"/>
-    </row>
-    <row r="23" spans="1:26">
-      <c r="A23" s="15"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="39" t="str">
+      <c r="P22" s="77"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="78"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="78"/>
+      <c r="W22" s="78"/>
+      <c r="X22" s="78"/>
+      <c r="Y22" s="78"/>
+      <c r="Z22" s="78"/>
+    </row>
+    <row r="23" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="71"/>
+      <c r="B23" s="30">
+        <v>6</v>
+      </c>
+      <c r="C23" s="99" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="42">
+        <v>6</v>
+      </c>
+      <c r="G23" s="43">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="H23" s="44">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="I23" s="45">
+        <v>0.51597222222222217</v>
+      </c>
+      <c r="J23" s="35">
+        <f t="shared" si="0"/>
+        <v>2.0833333333332149E-3</v>
+      </c>
+      <c r="K23" s="46">
+        <v>1</v>
+      </c>
+      <c r="L23" s="80">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M23" s="48">
+        <v>5</v>
+      </c>
+      <c r="N23" s="39">
+        <f t="shared" ref="N23:N25" si="2">IFERROR(IF(OR(J23="",ISBLANK(L23)),"",J23+L23),"Error")</f>
+        <v>2.7777777777776595E-3</v>
+      </c>
+      <c r="O23" s="71"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="78"/>
+      <c r="T23" s="78"/>
+      <c r="U23" s="78"/>
+      <c r="V23" s="78"/>
+      <c r="W23" s="78"/>
+      <c r="X23" s="78"/>
+      <c r="Y23" s="78"/>
+      <c r="Z23" s="78"/>
+    </row>
+    <row r="24" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="71"/>
+      <c r="B24" s="30">
+        <v>7</v>
+      </c>
+      <c r="C24" s="99" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="94"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="42">
+        <v>50</v>
+      </c>
+      <c r="G24" s="43">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H24" s="44">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="I24" s="45">
+        <v>0.53125</v>
+      </c>
+      <c r="J24" s="35">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="K24" s="46">
+        <v>2</v>
+      </c>
+      <c r="L24" s="80">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M24" s="48">
+        <v>25</v>
+      </c>
+      <c r="N24" s="39">
+        <f t="shared" si="2"/>
+        <v>1.7361111111111074E-2</v>
+      </c>
+      <c r="O24" s="71"/>
+      <c r="P24" s="77"/>
+      <c r="Q24" s="78"/>
+      <c r="R24" s="78"/>
+      <c r="S24" s="78"/>
+      <c r="T24" s="78"/>
+      <c r="U24" s="78"/>
+      <c r="V24" s="78"/>
+      <c r="W24" s="78"/>
+      <c r="X24" s="78"/>
+      <c r="Y24" s="78"/>
+      <c r="Z24" s="78"/>
+    </row>
+    <row r="25" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
+      <c r="A25" s="71"/>
+      <c r="B25" s="30">
+        <v>8</v>
+      </c>
+      <c r="C25" s="99"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="39" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="O23" s="15"/>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="22"/>
-      <c r="W23" s="22"/>
-      <c r="X23" s="22"/>
-      <c r="Y23" s="22"/>
-      <c r="Z23" s="22"/>
-    </row>
-    <row r="24" spans="1:26">
-      <c r="A24" s="15"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="39" t="str">
-        <f t="shared" si="2"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="77"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
+      <c r="U25" s="78"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="A26" s="15"/>
+      <c r="B26" s="30">
+        <v>9</v>
+      </c>
+      <c r="C26" s="99"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="39" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="O24" s="15"/>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="22"/>
-      <c r="X24" s="22"/>
-      <c r="Y24" s="22"/>
-      <c r="Z24" s="22"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" s="88" t="s">
+      <c r="O26" s="15"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22"/>
+      <c r="Z26" s="22"/>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27" s="15"/>
+      <c r="B27" s="30">
+        <v>10</v>
+      </c>
+      <c r="C27" s="99"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O27" s="15"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A28" s="7"/>
+      <c r="B28" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="49">
-        <f>IF(SUM(F18:F24)=0,"Completar",SUM(F18:F24))</f>
-        <v>155</v>
+      <c r="C28" s="125"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="49">
+        <f>IF(SUM(F18:F27)=0,"Completar",SUM(F18:F27))</f>
+        <v>211</v>
       </c>
-      <c r="G25" s="50">
-        <f>IF(SUM(G18:G24)=0,"Completar",SUM(G18:G24))</f>
-        <v>9.7222222222222224E-2</v>
+      <c r="G28" s="50">
+        <f>IF(SUM(G18:G27)=0,"Completar",SUM(G18:G27))</f>
+        <v>0.11458333333333334</v>
       </c>
-      <c r="H25" s="51" t="s">
+      <c r="H28" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="52" t="s">
+      <c r="I28" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="53">
-        <f>IF(OR(COUNTIF(J18:J24,"Error")&gt;0,COUNTIF(J18:J24,"Completar")&gt;0),"Error",IF(SUM(J18:J24)=0,"Completar",SUM(J18:J24)))</f>
-        <v>8.2638888888888928E-2</v>
+      <c r="J28" s="53">
+        <f>IF(OR(COUNTIF(J18:J27,"Error")&gt;0,COUNTIF(J18:J27,"Completar")&gt;0),"Error",IF(SUM(J18:J27)=0,"Completar",SUM(J18:J27)))</f>
+        <v>9.5138888888888773E-2</v>
       </c>
-      <c r="K25" s="54">
-        <f>SUM(K18:K24)</f>
+      <c r="K28" s="54">
+        <f>SUM(K18:K27)</f>
+        <v>5</v>
+      </c>
+      <c r="L28" s="50">
+        <f>SUM(L18:L27)</f>
+        <v>2.1527777777777778E-2</v>
+      </c>
+      <c r="M28" s="55">
+        <f>IF(SUM(M18:M27)=0,"Completar",SUM(M18:M27))</f>
+        <v>120</v>
+      </c>
+      <c r="N28" s="18">
+        <f>IF(OR(COUNTIF(N18:N27,"Error")&gt;0,COUNTIF(N18:N27,"Completar")&gt;0),"Error",IF(SUM(N18:N27)=0,"Completar",SUM(N18:N27)))</f>
+        <v>0.11666666666666656</v>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
+      <c r="V28" s="57"/>
+      <c r="W28" s="57"/>
+      <c r="X28" s="57"/>
+      <c r="Y28" s="57"/>
+      <c r="Z28" s="57"/>
+    </row>
+    <row r="29" spans="1:26" ht="6" customHeight="1">
+      <c r="A29" s="20"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+    </row>
+    <row r="30" spans="1:26" ht="15" customHeight="1">
+      <c r="A30" s="4"/>
+      <c r="B30" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="123"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="124"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+    </row>
+    <row r="31" spans="1:26" ht="30" customHeight="1">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L25" s="50">
-        <f>SUM(L18:L24)</f>
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="M25" s="55">
-        <f>IF(SUM(M18:M24)=0,"Completar",SUM(M18:M24))</f>
-        <v>98</v>
-      </c>
-      <c r="N25" s="18">
-        <f>IF(OR(COUNTIF(N18:N24,"Error")&gt;0,COUNTIF(N18:N24,"Completar")&gt;0),"Error",IF(SUM(N18:N24)=0,"Completar",SUM(N18:N24)))</f>
-        <v>9.6527777777777823E-2</v>
-      </c>
-      <c r="O25" s="7"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="57"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="57"/>
-      <c r="U25" s="57"/>
-      <c r="V25" s="57"/>
-      <c r="W25" s="57"/>
-      <c r="X25" s="57"/>
-      <c r="Y25" s="57"/>
-      <c r="Z25" s="57"/>
-    </row>
-    <row r="26" spans="1:26" ht="6" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="23"/>
-      <c r="Z26" s="23"/>
-    </row>
-    <row r="27" spans="1:26" ht="15" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="85" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-    </row>
-    <row r="28" spans="1:26" ht="30" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="14"/>
-      <c r="Y28" s="14"/>
-      <c r="Z28" s="14"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A29" s="15"/>
-      <c r="B29" s="58">
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A32" s="15"/>
+      <c r="B32" s="58">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C32" s="25">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D32" s="25">
         <v>0.36249999999999999</v>
       </c>
-      <c r="E29" s="18">
-        <f>IFERROR(IF(OR(ISBLANK(C29),ISBLANK(D29)),"Completar",IF(D29&gt;=C29,D29-C29,"Error")),"Error")</f>
+      <c r="E32" s="18">
+        <f>IFERROR(IF(OR(ISBLANK(C32),ISBLANK(D32)),"Completar",IF(D32&gt;=C32,D32-C32,"Error")),"Error")</f>
         <v>2.9166666666666674E-2</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="22"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22"/>
-      <c r="Z29" s="22"/>
-    </row>
-    <row r="30" spans="1:26" ht="6" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="23"/>
-      <c r="Y30" s="23"/>
-      <c r="Z30" s="23"/>
-    </row>
-    <row r="31" spans="1:26">
-      <c r="A31" s="20"/>
-      <c r="B31" s="85" t="s">
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="22"/>
+    </row>
+    <row r="33" spans="1:26" ht="6" customHeight="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="23"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="23"/>
+    </row>
+    <row r="34" spans="1:26">
+      <c r="A34" s="20"/>
+      <c r="B34" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="86"/>
-      <c r="M31" s="86"/>
-      <c r="N31" s="87"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
-      <c r="R31" s="59"/>
-      <c r="S31" s="59"/>
-      <c r="T31" s="59"/>
-      <c r="U31" s="59"/>
-      <c r="V31" s="59"/>
-      <c r="W31" s="59"/>
-      <c r="X31" s="59"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="59"/>
-    </row>
-    <row r="32" spans="1:26" ht="15" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="107" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="91"/>
-      <c r="D32" s="108"/>
-      <c r="E32" s="109">
-        <f>M25</f>
-        <v>98</v>
-      </c>
-      <c r="F32" s="108"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
-      <c r="N32" s="62"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-      <c r="R32" s="59"/>
-      <c r="S32" s="59"/>
-      <c r="T32" s="59"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="59"/>
-      <c r="W32" s="59"/>
-      <c r="X32" s="59"/>
-      <c r="Y32" s="59"/>
-      <c r="Z32" s="59"/>
-    </row>
-    <row r="33" spans="1:26">
-      <c r="A33" s="20"/>
-      <c r="B33" s="107" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="91"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="117">
-        <f>IF(M25="Completar","Completar",IFERROR(M25/(N25*24),"Error"))</f>
-        <v>42.302158273381274</v>
-      </c>
-      <c r="F33" s="108"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="59"/>
-      <c r="R33" s="59"/>
-      <c r="S33" s="59"/>
-      <c r="T33" s="59"/>
-      <c r="U33" s="59"/>
-      <c r="V33" s="59"/>
-      <c r="W33" s="59"/>
-      <c r="X33" s="59"/>
-      <c r="Y33" s="59"/>
-      <c r="Z33" s="59"/>
-    </row>
-    <row r="34" spans="1:26" ht="15" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="107" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="91"/>
-      <c r="D34" s="108"/>
-      <c r="E34" s="109">
-        <f>IF(K25=0,0,IFERROR(ROUNDUP(K25/(M25/100),0),"Error"))</f>
-        <v>3</v>
-      </c>
-      <c r="F34" s="108"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="65"/>
+      <c r="C34" s="123"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="123"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="123"/>
+      <c r="H34" s="123"/>
+      <c r="I34" s="123"/>
+      <c r="J34" s="123"/>
+      <c r="K34" s="123"/>
+      <c r="L34" s="123"/>
+      <c r="M34" s="123"/>
+      <c r="N34" s="124"/>
       <c r="O34" s="20"/>
       <c r="P34" s="59"/>
       <c r="Q34" s="59"/>
@@ -2912,24 +2988,24 @@
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1">
       <c r="A35" s="20"/>
-      <c r="B35" s="107" t="s">
-        <v>28</v>
+      <c r="B35" s="93" t="s">
+        <v>25</v>
       </c>
-      <c r="C35" s="91"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="116">
-        <f>IF(K25=0,0,IFERROR(K25/M25,"Error"))</f>
-        <v>2.0408163265306121E-2</v>
+      <c r="C35" s="121"/>
+      <c r="D35" s="122"/>
+      <c r="E35" s="102">
+        <f>M28</f>
+        <v>120</v>
       </c>
-      <c r="F35" s="108"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="64"/>
-      <c r="K35" s="64"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="64"/>
-      <c r="N35" s="65"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="62"/>
       <c r="O35" s="20"/>
       <c r="P35" s="59"/>
       <c r="Q35" s="59"/>
@@ -2943,21 +3019,18 @@
       <c r="Y35" s="59"/>
       <c r="Z35" s="59"/>
     </row>
-    <row r="36" spans="1:26" ht="15" customHeight="1">
+    <row r="36" spans="1:26">
       <c r="A36" s="20"/>
-      <c r="B36" s="107" t="s">
-        <v>29</v>
+      <c r="B36" s="93" t="s">
+        <v>26</v>
       </c>
-      <c r="C36" s="91"/>
-      <c r="D36" s="108"/>
-      <c r="E36" s="66">
-        <f>E5</f>
-        <v>1.1805555555555569E-2</v>
+      <c r="C36" s="121"/>
+      <c r="D36" s="122"/>
+      <c r="E36" s="101">
+        <f>IF(M28="Completar","Completar",IFERROR(M28/(N28*24),"Error"))</f>
+        <v>42.857142857142904</v>
       </c>
-      <c r="F36" s="67">
-        <f t="shared" ref="F36:F39" si="3">IF(E36="Completar",E36,IFERROR(E36/$E$42,"Error"))</f>
-        <v>4.096385542168679E-2</v>
-      </c>
+      <c r="F36" s="95"/>
       <c r="G36" s="63"/>
       <c r="H36" s="64"/>
       <c r="I36" s="64"/>
@@ -2981,19 +3054,16 @@
     </row>
     <row r="37" spans="1:26" ht="15" customHeight="1">
       <c r="A37" s="20"/>
-      <c r="B37" s="107" t="s">
-        <v>30</v>
+      <c r="B37" s="93" t="s">
+        <v>27</v>
       </c>
-      <c r="C37" s="91"/>
-      <c r="D37" s="108"/>
-      <c r="E37" s="66">
-        <f>E9</f>
-        <v>0.13888888888888884</v>
+      <c r="C37" s="121"/>
+      <c r="D37" s="122"/>
+      <c r="E37" s="102">
+        <f>IF(K28=0,0,IFERROR(ROUNDUP(K28/(M28/100),0),"Error"))</f>
+        <v>5</v>
       </c>
-      <c r="F37" s="67">
-        <f t="shared" si="3"/>
-        <v>0.48192771084337327</v>
-      </c>
+      <c r="F37" s="95"/>
       <c r="G37" s="63"/>
       <c r="H37" s="64"/>
       <c r="I37" s="64"/>
@@ -3017,19 +3087,16 @@
     </row>
     <row r="38" spans="1:26" ht="15" customHeight="1">
       <c r="A38" s="20"/>
-      <c r="B38" s="107" t="s">
-        <v>31</v>
+      <c r="B38" s="93" t="s">
+        <v>28</v>
       </c>
-      <c r="C38" s="91"/>
-      <c r="D38" s="108"/>
-      <c r="E38" s="66">
-        <f>E13</f>
-        <v>1.1805555555555569E-2</v>
+      <c r="C38" s="121"/>
+      <c r="D38" s="122"/>
+      <c r="E38" s="100">
+        <f>IF(K28=0,0,IFERROR(K28/M28,"Error"))</f>
+        <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F38" s="67">
-        <f t="shared" si="3"/>
-        <v>4.096385542168679E-2</v>
-      </c>
+      <c r="F38" s="95"/>
       <c r="G38" s="63"/>
       <c r="H38" s="64"/>
       <c r="I38" s="64"/>
@@ -3053,18 +3120,18 @@
     </row>
     <row r="39" spans="1:26" ht="15" customHeight="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="107" t="s">
-        <v>32</v>
+      <c r="B39" s="93" t="s">
+        <v>29</v>
       </c>
-      <c r="C39" s="91"/>
-      <c r="D39" s="108"/>
+      <c r="C39" s="121"/>
+      <c r="D39" s="122"/>
       <c r="E39" s="66">
-        <f>E29</f>
-        <v>2.9166666666666674E-2</v>
+        <f>E5</f>
+        <v>1.1805555555555569E-2</v>
       </c>
       <c r="F39" s="67">
-        <f t="shared" si="3"/>
-        <v>0.10120481927710845</v>
+        <f t="shared" ref="F39:F42" si="3">IF(E39="Completar",E39,IFERROR(E39/$E$45,"Error"))</f>
+        <v>3.8288288288288341E-2</v>
       </c>
       <c r="G39" s="63"/>
       <c r="H39" s="64"/>
@@ -3089,18 +3156,18 @@
     </row>
     <row r="40" spans="1:26" ht="15" customHeight="1">
       <c r="A40" s="20"/>
-      <c r="B40" s="107" t="s">
-        <v>33</v>
+      <c r="B40" s="93" t="s">
+        <v>30</v>
       </c>
-      <c r="C40" s="91"/>
-      <c r="D40" s="108"/>
+      <c r="C40" s="121"/>
+      <c r="D40" s="122"/>
       <c r="E40" s="66">
-        <f>L25</f>
-        <v>1.3888888888888888E-2</v>
+        <f>E9</f>
+        <v>0.13888888888888884</v>
       </c>
       <c r="F40" s="67">
-        <f t="shared" ref="F40:F41" si="4">IF(E40="Completar",E40,IFERROR(E40/$E$42,"Completar"))</f>
-        <v>4.8192771084337345E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.45045045045045046</v>
       </c>
       <c r="G40" s="63"/>
       <c r="H40" s="64"/>
@@ -3125,18 +3192,18 @@
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1">
       <c r="A41" s="20"/>
-      <c r="B41" s="107" t="s">
-        <v>34</v>
+      <c r="B41" s="93" t="s">
+        <v>31</v>
       </c>
-      <c r="C41" s="91"/>
-      <c r="D41" s="108"/>
+      <c r="C41" s="121"/>
+      <c r="D41" s="122"/>
       <c r="E41" s="66">
-        <f>J25</f>
-        <v>8.2638888888888928E-2</v>
+        <f>E13</f>
+        <v>1.1805555555555569E-2</v>
       </c>
       <c r="F41" s="67">
-        <f t="shared" si="4"/>
-        <v>0.28674698795180731</v>
+        <f t="shared" si="3"/>
+        <v>3.8288288288288341E-2</v>
       </c>
       <c r="G41" s="63"/>
       <c r="H41" s="64"/>
@@ -3161,24 +3228,27 @@
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="115" t="s">
-        <v>35</v>
+      <c r="B42" s="93" t="s">
+        <v>32</v>
       </c>
-      <c r="C42" s="89"/>
-      <c r="D42" s="114"/>
-      <c r="E42" s="113">
-        <f>IF(COUNTIF(E36:E41,"Error")&gt;0,"Error",IF(SUM(E36:E41)=0,"Completar",SUM(E36:E41)))</f>
-        <v>0.28819444444444448</v>
+      <c r="C42" s="121"/>
+      <c r="D42" s="122"/>
+      <c r="E42" s="66">
+        <f>E32</f>
+        <v>2.9166666666666674E-2</v>
       </c>
-      <c r="F42" s="114"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="70"/>
+      <c r="F42" s="67">
+        <f t="shared" si="3"/>
+        <v>9.4594594594594641E-2</v>
+      </c>
+      <c r="G42" s="63"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="64"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="64"/>
+      <c r="N42" s="65"/>
       <c r="O42" s="20"/>
       <c r="P42" s="59"/>
       <c r="Q42" s="59"/>
@@ -3192,49 +3262,65 @@
       <c r="Y42" s="59"/>
       <c r="Z42" s="59"/>
     </row>
-    <row r="43" spans="1:26" ht="6" customHeight="1">
+    <row r="43" spans="1:26" ht="15" customHeight="1">
       <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
+      <c r="B43" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="121"/>
+      <c r="D43" s="122"/>
+      <c r="E43" s="66">
+        <f>L28</f>
+        <v>2.1527777777777778E-2</v>
+      </c>
+      <c r="F43" s="67">
+        <f t="shared" ref="F43:F44" si="4">IF(E43="Completar",E43,IFERROR(E43/$E$45,"Completar"))</f>
+        <v>6.9819819819819842E-2</v>
+      </c>
+      <c r="G43" s="63"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="64"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="64"/>
+      <c r="N43" s="65"/>
       <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
-      <c r="S43" s="20"/>
-      <c r="T43" s="20"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
-      <c r="X43" s="20"/>
-      <c r="Y43" s="20"/>
-      <c r="Z43" s="20"/>
-    </row>
-    <row r="44" spans="1:26" hidden="1">
+      <c r="P43" s="59"/>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="59"/>
+      <c r="S43" s="59"/>
+      <c r="T43" s="59"/>
+      <c r="U43" s="59"/>
+      <c r="V43" s="59"/>
+      <c r="W43" s="59"/>
+      <c r="X43" s="59"/>
+      <c r="Y43" s="59"/>
+      <c r="Z43" s="59"/>
+    </row>
+    <row r="44" spans="1:26" ht="15" customHeight="1">
       <c r="A44" s="20"/>
-      <c r="B44" s="59"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
-      <c r="K44" s="59"/>
-      <c r="L44" s="59"/>
-      <c r="M44" s="59"/>
-      <c r="N44" s="59"/>
+      <c r="B44" s="93" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="121"/>
+      <c r="D44" s="122"/>
+      <c r="E44" s="66">
+        <f>J28</f>
+        <v>9.5138888888888773E-2</v>
+      </c>
+      <c r="F44" s="67">
+        <f t="shared" si="4"/>
+        <v>0.30855855855855829</v>
+      </c>
+      <c r="G44" s="63"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="64"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64"/>
+      <c r="N44" s="65"/>
       <c r="O44" s="20"/>
       <c r="P44" s="59"/>
       <c r="Q44" s="59"/>
@@ -3248,21 +3334,26 @@
       <c r="Y44" s="59"/>
       <c r="Z44" s="59"/>
     </row>
-    <row r="45" spans="1:26">
+    <row r="45" spans="1:26" ht="15" customHeight="1">
       <c r="A45" s="20"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="59"/>
-      <c r="L45" s="59"/>
-      <c r="M45" s="59"/>
-      <c r="N45" s="59"/>
+      <c r="B45" s="98" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="119"/>
+      <c r="D45" s="120"/>
+      <c r="E45" s="96">
+        <f>IF(COUNTIF(E39:E44,"Error")&gt;0,"Error",IF(SUM(E39:E44)=0,"Completar",SUM(E39:E44)))</f>
+        <v>0.30833333333333324</v>
+      </c>
+      <c r="F45" s="97"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="69"/>
+      <c r="K45" s="69"/>
+      <c r="L45" s="69"/>
+      <c r="M45" s="69"/>
+      <c r="N45" s="70"/>
       <c r="O45" s="20"/>
       <c r="P45" s="59"/>
       <c r="Q45" s="59"/>
@@ -3276,35 +3367,35 @@
       <c r="Y45" s="59"/>
       <c r="Z45" s="59"/>
     </row>
-    <row r="46" spans="1:26">
+    <row r="46" spans="1:26" ht="6" customHeight="1">
       <c r="A46" s="20"/>
-      <c r="B46" s="59"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
-      <c r="L46" s="59"/>
-      <c r="M46" s="59"/>
-      <c r="N46" s="59"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
       <c r="O46" s="20"/>
-      <c r="P46" s="59"/>
-      <c r="Q46" s="59"/>
-      <c r="R46" s="59"/>
-      <c r="S46" s="59"/>
-      <c r="T46" s="59"/>
-      <c r="U46" s="59"/>
-      <c r="V46" s="59"/>
-      <c r="W46" s="59"/>
-      <c r="X46" s="59"/>
-      <c r="Y46" s="59"/>
-      <c r="Z46" s="59"/>
-    </row>
-    <row r="47" spans="1:26">
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="20"/>
+      <c r="S46" s="20"/>
+      <c r="T46" s="20"/>
+      <c r="U46" s="20"/>
+      <c r="V46" s="20"/>
+      <c r="W46" s="20"/>
+      <c r="X46" s="20"/>
+      <c r="Y46" s="20"/>
+      <c r="Z46" s="20"/>
+    </row>
+    <row r="47" spans="1:26" hidden="1">
       <c r="A47" s="20"/>
       <c r="B47" s="59"/>
       <c r="C47" s="59"/>
@@ -29988,8 +30079,131 @@
       <c r="Y999" s="59"/>
       <c r="Z999" s="59"/>
     </row>
+    <row r="1000" spans="1:26">
+      <c r="A1000" s="20"/>
+      <c r="B1000" s="59"/>
+      <c r="C1000" s="59"/>
+      <c r="D1000" s="59"/>
+      <c r="E1000" s="59"/>
+      <c r="F1000" s="59"/>
+      <c r="G1000" s="59"/>
+      <c r="H1000" s="59"/>
+      <c r="I1000" s="59"/>
+      <c r="J1000" s="59"/>
+      <c r="K1000" s="59"/>
+      <c r="L1000" s="59"/>
+      <c r="M1000" s="59"/>
+      <c r="N1000" s="59"/>
+      <c r="O1000" s="20"/>
+      <c r="P1000" s="59"/>
+      <c r="Q1000" s="59"/>
+      <c r="R1000" s="59"/>
+      <c r="S1000" s="59"/>
+      <c r="T1000" s="59"/>
+      <c r="U1000" s="59"/>
+      <c r="V1000" s="59"/>
+      <c r="W1000" s="59"/>
+      <c r="X1000" s="59"/>
+      <c r="Y1000" s="59"/>
+      <c r="Z1000" s="59"/>
+    </row>
+    <row r="1001" spans="1:26">
+      <c r="A1001" s="20"/>
+      <c r="B1001" s="59"/>
+      <c r="C1001" s="59"/>
+      <c r="D1001" s="59"/>
+      <c r="E1001" s="59"/>
+      <c r="F1001" s="59"/>
+      <c r="G1001" s="59"/>
+      <c r="H1001" s="59"/>
+      <c r="I1001" s="59"/>
+      <c r="J1001" s="59"/>
+      <c r="K1001" s="59"/>
+      <c r="L1001" s="59"/>
+      <c r="M1001" s="59"/>
+      <c r="N1001" s="59"/>
+      <c r="O1001" s="20"/>
+      <c r="P1001" s="59"/>
+      <c r="Q1001" s="59"/>
+      <c r="R1001" s="59"/>
+      <c r="S1001" s="59"/>
+      <c r="T1001" s="59"/>
+      <c r="U1001" s="59"/>
+      <c r="V1001" s="59"/>
+      <c r="W1001" s="59"/>
+      <c r="X1001" s="59"/>
+      <c r="Y1001" s="59"/>
+      <c r="Z1001" s="59"/>
+    </row>
+    <row r="1002" spans="1:26">
+      <c r="A1002" s="20"/>
+      <c r="B1002" s="59"/>
+      <c r="C1002" s="59"/>
+      <c r="D1002" s="59"/>
+      <c r="E1002" s="59"/>
+      <c r="F1002" s="59"/>
+      <c r="G1002" s="59"/>
+      <c r="H1002" s="59"/>
+      <c r="I1002" s="59"/>
+      <c r="J1002" s="59"/>
+      <c r="K1002" s="59"/>
+      <c r="L1002" s="59"/>
+      <c r="M1002" s="59"/>
+      <c r="N1002" s="59"/>
+      <c r="O1002" s="20"/>
+      <c r="P1002" s="59"/>
+      <c r="Q1002" s="59"/>
+      <c r="R1002" s="59"/>
+      <c r="S1002" s="59"/>
+      <c r="T1002" s="59"/>
+      <c r="U1002" s="59"/>
+      <c r="V1002" s="59"/>
+      <c r="W1002" s="59"/>
+      <c r="X1002" s="59"/>
+      <c r="Y1002" s="59"/>
+      <c r="Z1002" s="59"/>
+    </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="46">
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B34:N34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="D1:N1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B7:E7"/>
@@ -29997,49 +30211,13 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B31:N31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B25:E25"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C24 A25:XFD1048576 A1:B24 D1:XFD24 C22:E22">
+  <conditionalFormatting sqref="C3:C22 D1:XFD22 C22:E22 A28:XFD1048576 C23:XFD27 A1:B27">
     <cfRule type="cellIs" dxfId="1" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C24 A25:XFD1048576 A1:B24 D1:XFD24 C22:E22">
+  <conditionalFormatting sqref="C3:C22 D1:XFD22 C22:E22 A28:XFD1048576 C23:XFD27 A1:B27">
     <cfRule type="cellIs" dxfId="0" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>

</xml_diff>